<commit_message>
it asked me to save when i quit fsr so i saved
</commit_message>
<xml_diff>
--- a/list of lpl videos sorted by length.xlsx
+++ b/list of lpl videos sorted by length.xlsx
@@ -7461,8 +7461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A1379" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24293,7 +24293,7 @@
   <dimension ref="A1:I8400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4930" sqref="A4930"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>